<commit_message>
Switch updated, Excel BOM complete
</commit_message>
<xml_diff>
--- a/V1/CabinTempSenseHardware/CabinTempSenseHardware.xlsx
+++ b/V1/CabinTempSenseHardware/CabinTempSenseHardware.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Part</t>
   </si>
@@ -47,9 +47,6 @@
     <t>0603 Capacitor</t>
   </si>
   <si>
-    <t>100 uF</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -134,20 +131,106 @@
     <t>Recom RO Series 1W DCDC</t>
   </si>
   <si>
-    <t>LDO</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
     <t>U4</t>
+  </si>
+  <si>
+    <t>0603 Resistor</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <r>
+      <t>120</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>12 - 5V</t>
+  </si>
+  <si>
+    <t>5 - 3.3V</t>
+  </si>
+  <si>
+    <t>http://www.digikey.ca/product-detail/en/stmicroelectronics/STM32F103C4T6A/497-8316-ND/1956095</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/recom-power/R-78E5.0-0.5/945-1648-5-ND/2834904</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/recom-power/RO-053.3S/945-1524-5-ND/2314958</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/molex-llc/0430450623/WM14569-ND/3310197</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/microchip-technology/MCP2562T-E-SN/MCP2562T-E-SNTR-ND/4079891</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/yageo/RC0603JR-07120RL/311-120GRTR-ND/726706</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/murata-electronics-north-america/GRM188R71C105KE15J/490-14640-1-ND/6606246</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/yageo/CC0603KRX7R6BB334/311-3368-1-ND/6818338</t>
+  </si>
+  <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/murata-electronics-north-america/GCM188R71H103JA37D/490-14356-1-ND/6606817</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/products/en?keywords=CDSOD323-T03SCCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/products/en?keywords=CKN9085CT-ND</t>
+  </si>
+  <si>
+    <t>Per Board</t>
+  </si>
+  <si>
+    <t>Have on Hand</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/yageo/RC0603JR-07120RL/311-120GRCT-ND/729653</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/yageo/RC0603JR-074K7L/311-4.7KGRCT-ND/729732</t>
+  </si>
+  <si>
+    <t>Order Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +242,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,14 +278,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,8 +615,8 @@
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="97.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="108.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -536,13 +636,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -550,13 +650,26 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2">
         <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2">
+        <f>F2*E2</f>
+        <v>0.73</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -564,13 +677,25 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3">
+        <v>0.16</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -578,132 +703,358 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4">
+        <f>E4*F4</f>
+        <v>0.53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5">
+        <f>E5*F5</f>
+        <v>7.78</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
       <c r="D6">
         <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3.65</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6">
+        <f>E6*F6</f>
+        <v>10.95</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
       <c r="D7">
         <v>1</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0.32</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7">
+        <f>E7*F7</f>
+        <v>0.96</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
       <c r="D8">
         <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>1.07</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <f>E8*F8</f>
+        <v>3.21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
       <c r="D9">
         <v>1</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>7.46</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9">
+        <f>E9*F9</f>
+        <v>37.299999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
-        <v>30</v>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>1.78</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10">
+        <f>E10*F10</f>
+        <v>8.9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11">
+        <v>4.08</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>7.72</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <f>E12*F12</f>
+        <v>23.16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="D12">
-        <v>1</v>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1000</v>
+      </c>
+      <c r="F13">
+        <v>2.7599999999999999E-3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13">
+        <f>E13*F13</f>
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14">
+        <v>2.7599999999999999E-3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15">
+        <v>2.7599999999999999E-3</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <f>D2*F2+D3*F3+D4*F4+D5*F5+D6*F6+D7*F7+D8*F8+D9*F9+D10*F10+D11*F11+D12*F12+D13*F13+D14*F14+D15*F15</f>
+        <v>28.253039999999995</v>
+      </c>
+      <c r="H17">
+        <f>H2+H3+H4+H5+H6+H7+H8+H9+H10+H11+H12+H13+H14+H15</f>
+        <v>96.28</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G13" r:id="rId1"/>
+    <hyperlink ref="G12" r:id="rId2"/>
+    <hyperlink ref="G11" r:id="rId3"/>
+    <hyperlink ref="G10" r:id="rId4"/>
+    <hyperlink ref="G9" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G6" r:id="rId7"/>
+    <hyperlink ref="G14" r:id="rId8"/>
+    <hyperlink ref="G15" r:id="rId9"/>
+    <hyperlink ref="G4" r:id="rId10"/>
+    <hyperlink ref="G3" r:id="rId11"/>
+    <hyperlink ref="G2" r:id="rId12"/>
+    <hyperlink ref="G5" r:id="rId13"/>
+    <hyperlink ref="G7" r:id="rId14"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel and BOM updated
</commit_message>
<xml_diff>
--- a/V1/CabinTempSenseHardware/CabinTempSenseHardware.xlsx
+++ b/V1/CabinTempSenseHardware/CabinTempSenseHardware.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Part</t>
   </si>
@@ -224,6 +224,18 @@
   </si>
   <si>
     <t>Order Total</t>
+  </si>
+  <si>
+    <t>ON Schottky Diode</t>
+  </si>
+  <si>
+    <t>MBRM110LT1G</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/on-semiconductor/MBRM110LT1G/MBRM110LT1GOSCT-ND/917992</t>
   </si>
 </sst>
 </file>
@@ -601,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +733,7 @@
         <v>52</v>
       </c>
       <c r="H4">
-        <f>E4*F4</f>
+        <f t="shared" ref="H4:H10" si="0">E4*F4</f>
         <v>0.53</v>
       </c>
     </row>
@@ -748,7 +760,7 @@
         <v>56</v>
       </c>
       <c r="H5">
-        <f>E5*F5</f>
+        <f t="shared" si="0"/>
         <v>7.78</v>
       </c>
     </row>
@@ -775,7 +787,7 @@
         <v>49</v>
       </c>
       <c r="H6">
-        <f>E6*F6</f>
+        <f t="shared" si="0"/>
         <v>10.95</v>
       </c>
     </row>
@@ -802,7 +814,7 @@
         <v>57</v>
       </c>
       <c r="H7">
-        <f>E7*F7</f>
+        <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
     </row>
@@ -829,7 +841,7 @@
         <v>50</v>
       </c>
       <c r="H8">
-        <f>E8*F8</f>
+        <f t="shared" si="0"/>
         <v>3.21</v>
       </c>
     </row>
@@ -856,7 +868,7 @@
         <v>46</v>
       </c>
       <c r="H9">
-        <f>E9*F9</f>
+        <f t="shared" si="0"/>
         <v>37.299999999999997</v>
       </c>
     </row>
@@ -883,7 +895,7 @@
         <v>29</v>
       </c>
       <c r="H10">
-        <f>E10*F10</f>
+        <f t="shared" si="0"/>
         <v>8.9</v>
       </c>
     </row>
@@ -1020,21 +1032,48 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16">
+        <f>E16*F16</f>
+        <v>5.5400000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F17">
-        <f>D2*F2+D3*F3+D4*F4+D5*F5+D6*F6+D7*F7+D8*F8+D9*F9+D10*F10+D11*F11+D12*F12+D13*F13+D14*F14+D15*F15</f>
-        <v>28.253039999999995</v>
-      </c>
-      <c r="H17">
-        <f>H2+H3+H4+H5+H6+H7+H8+H9+H10+H11+H12+H13+H14+H15</f>
-        <v>96.28</v>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <f>D2*F2+D3*F3+D4*F4+D5*F5+D6*F6+D7*F7+D8*F8+D9*F9+D10*F10+D11*F11+D12*F12+D13*F13+D14*F14+D15*F15+D16*F16</f>
+        <v>28.807039999999994</v>
+      </c>
+      <c r="H18">
+        <f>H2+H3+H4+H5+H6+H7+H8+H9+H10+H11+H12+H13+H14+H15+H16</f>
+        <v>101.82000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1053,8 +1092,9 @@
     <hyperlink ref="G2" r:id="rId12"/>
     <hyperlink ref="G5" r:id="rId13"/>
     <hyperlink ref="G7" r:id="rId14"/>
+    <hyperlink ref="G16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Diode removed, more MCU caps added and shuffled around, Vias Everywheregit add -A
</commit_message>
<xml_diff>
--- a/V1/CabinTempSenseHardware/CabinTempSenseHardware.xlsx
+++ b/V1/CabinTempSenseHardware/CabinTempSenseHardware.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Part</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>C1</t>
-  </si>
-  <si>
-    <t>C2, C3, C4</t>
   </si>
   <si>
     <t>0.33uF</t>
@@ -226,16 +223,7 @@
     <t>Order Total</t>
   </si>
   <si>
-    <t>ON Schottky Diode</t>
-  </si>
-  <si>
-    <t>MBRM110LT1G</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/on-semiconductor/MBRM110LT1G/MBRM110LT1GOSCT-ND/917992</t>
+    <t>C2, C3, C4, C5, C6</t>
   </si>
 </sst>
 </file>
@@ -615,15 +603,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
@@ -648,13 +636,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -662,7 +650,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -677,7 +665,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2">
         <f>F2*E2</f>
@@ -689,22 +677,22 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3">
         <v>0.16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -715,10 +703,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -730,7 +718,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H10" si="0">E4*F4</f>
@@ -739,13 +727,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -757,7 +745,7 @@
         <v>0.77800000000000002</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
@@ -766,13 +754,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -784,7 +772,7 @@
         <v>3.65</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
@@ -793,13 +781,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -811,7 +799,7 @@
         <v>0.32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
@@ -820,13 +808,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -838,7 +826,7 @@
         <v>1.07</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
@@ -847,13 +835,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -865,7 +853,7 @@
         <v>7.46</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
@@ -874,13 +862,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -892,7 +880,7 @@
         <v>1.78</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
@@ -901,25 +889,25 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11">
         <v>4.08</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -927,13 +915,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -945,7 +933,7 @@
         <v>7.72</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12">
         <f>E12*F12</f>
@@ -954,13 +942,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -972,7 +960,7 @@
         <v>2.7599999999999999E-3</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13">
         <f>E13*F13</f>
@@ -981,25 +969,25 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14">
         <v>2.7599999999999999E-3</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1007,73 +995,49 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15">
         <v>2.7599999999999999E-3</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16">
-        <v>0.55400000000000005</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16">
-        <f>E16*F16</f>
-        <v>5.5400000000000009</v>
-      </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F18">
         <f>D2*F2+D3*F3+D4*F4+D5*F5+D6*F6+D7*F7+D8*F8+D9*F9+D10*F10+D11*F11+D12*F12+D13*F13+D14*F14+D15*F15+D16*F16</f>
-        <v>28.807039999999994</v>
+        <v>28.573039999999995</v>
       </c>
       <c r="H18">
         <f>H2+H3+H4+H5+H6+H7+H8+H9+H10+H11+H12+H13+H14+H15+H16</f>
-        <v>101.82000000000001</v>
+        <v>96.28</v>
       </c>
     </row>
   </sheetData>
@@ -1092,9 +1056,8 @@
     <hyperlink ref="G2" r:id="rId12"/>
     <hyperlink ref="G5" r:id="rId13"/>
     <hyperlink ref="G7" r:id="rId14"/>
-    <hyperlink ref="G16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId16"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added header, updated NC drill, imported newest changes to Altium
</commit_message>
<xml_diff>
--- a/V1/CabinTempSenseHardware/CabinTempSenseHardware.xlsx
+++ b/V1/CabinTempSenseHardware/CabinTempSenseHardware.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7632"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Part</t>
   </si>
@@ -225,11 +225,23 @@
   <si>
     <t>C2, C3, C4, C5, C6</t>
   </si>
+  <si>
+    <t>https://www.digikey.ca/products/en?keywords=%201175-1629-ND</t>
+  </si>
+  <si>
+    <t>ARM Cortex-M 10pin conn</t>
+  </si>
+  <si>
+    <t>10pin connector</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,11 +612,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,7 +1032,31 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G16" s="2"/>
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16">
+        <f>E16*F16</f>
+        <v>0.246</v>
+      </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
@@ -1033,29 +1069,29 @@
     <row r="18" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F18">
         <f>D2*F2+D3*F3+D4*F4+D5*F5+D6*F6+D7*F7+D8*F8+D9*F9+D10*F10+D11*F11+D12*F12+D13*F13+D14*F14+D15*F15+D16*F16</f>
-        <v>28.573039999999995</v>
+        <v>28.655039999999996</v>
       </c>
       <c r="H18">
         <f>H2+H3+H4+H5+H6+H7+H8+H9+H10+H11+H12+H13+H14+H15+H16</f>
-        <v>96.28</v>
+        <v>96.525999999999996</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G13" r:id="rId1"/>
-    <hyperlink ref="G12" r:id="rId2"/>
-    <hyperlink ref="G11" r:id="rId3"/>
-    <hyperlink ref="G10" r:id="rId4"/>
-    <hyperlink ref="G9" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G6" r:id="rId7"/>
-    <hyperlink ref="G14" r:id="rId8"/>
-    <hyperlink ref="G15" r:id="rId9"/>
-    <hyperlink ref="G4" r:id="rId10"/>
-    <hyperlink ref="G3" r:id="rId11"/>
-    <hyperlink ref="G2" r:id="rId12"/>
-    <hyperlink ref="G5" r:id="rId13"/>
-    <hyperlink ref="G7" r:id="rId14"/>
+    <hyperlink ref="G13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G11" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G3" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G2" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>

</xml_diff>